<commit_message>
Updated document revision history
</commit_message>
<xml_diff>
--- a/1.0/documents/JPCOARスキーマ項目一覧.xlsx
+++ b/1.0/documents/JPCOARスキーマ項目一覧.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22704448-05EB-4FFE-AF91-EECA859393D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D08752-90C9-4A35-AC94-0E357E76C7BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27555" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="10" r:id="rId1"/>
@@ -4146,25 +4146,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>■5 アクセス権 (dcterms:accessRights)
-　- 語彙の定義の追加
-■12 日付 (datacite:date)  / 35.4 日付 (datacite:date) 
-　- 語彙の説明を修正 (Available / Issued)
-　- 注意点の文面を修正
-■14 資源タイプ (dc:type)
-　- 語彙の名称変更 (learning material -&gt; learning object)および属性(rdf:resource)の変更
-　- 語彙の追加 (data management plan / interview / manuscript / newspaper / software paper)
-　- 注意点の文面を修正
-■34 会議記述 (jpcoar:conference)
-　- 34 .3 主催機関 (jpcoar:conferenceSponsor)、34 .4 開催期間 (jpcoar:conferenceDate)、34 .5 開催会場 (jpcoar:conferenceVenue)を追加
-　- 推奨例の修正
-■35 ファイル情報 (jpcoar:file) / 35.1 本文URL (jpcoar:URI)
-　- 語彙の追加 (dataset / software)
-　- 注意点の追加
-　- 推奨例の修正</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>JPCOARスキーマ項目一覧 ver.1.0.2</t>
     <rPh sb="10" eb="12">
       <t>コウモク</t>
@@ -4239,6 +4220,25 @@
 summary
 thumbnail
 other</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■5 アクセス権 (dcterms:accessRights)
+　- 語彙別表に解説を追加
+■12 日付 (datacite:date)  / 35.4 日付 (datacite:date) 
+　- 語彙の説明を修正 (Available / Issued)
+　- 注意点の文面を修正
+■14 資源タイプ (dc:type)
+　- 語彙の名称変更 (learning material -&gt; learning object)および属性(rdf:resource)の変更
+　- 語彙の追加 (data management plan / interview / manuscript / newspaper / software paper)
+　- 注意点の文面を修正
+■34 会議記述 (jpcoar:conference)
+　- 34 .3 主催機関 (jpcoar:conferenceSponsor)、34 .4 開催期間 (jpcoar:conferenceDate)、34 .5 開催会場 (jpcoar:conferenceVenue)を追加
+　- 推奨例の修正
+■35 ファイル情報 (jpcoar:file) / 35.1 本文URL (jpcoar:URI)
+　- 語彙の追加 (dataset / software)
+　- 注意点の追加
+　- 推奨例の修正</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5845,7 +5845,7 @@
     </row>
     <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="150" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C8" s="150"/>
       <c r="D8" s="150"/>
@@ -5944,8 +5944,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.875" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -6009,13 +6009,13 @@
         <v>43796</v>
       </c>
       <c r="C6" s="84" t="s">
-        <v>1138</v>
+        <v>1146</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7182,7 +7182,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7305,7 +7305,7 @@
         <v>56</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P2" s="23" t="s">
         <v>57</v>
@@ -9010,7 +9010,7 @@
         <v>243</v>
       </c>
       <c r="N47" s="158" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O47" s="158" t="s">
         <v>244</v>
@@ -11054,7 +11054,7 @@
         <v>509</v>
       </c>
       <c r="O98" s="23" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="P98" s="23"/>
       <c r="Q98" s="33"/>
@@ -11585,13 +11585,13 @@
         <v>88</v>
       </c>
       <c r="M113" s="158" t="s">
+        <v>1142</v>
+      </c>
+      <c r="N113" s="158" t="s">
         <v>1143</v>
       </c>
-      <c r="N113" s="158" t="s">
+      <c r="O113" s="158" t="s">
         <v>1144</v>
-      </c>
-      <c r="O113" s="158" t="s">
-        <v>1145</v>
       </c>
       <c r="P113" s="158"/>
       <c r="Q113" s="30"/>
@@ -11626,7 +11626,7 @@
       <c r="O114" s="162"/>
       <c r="P114" s="162"/>
       <c r="Q114" s="30" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="R114" s="4"/>
       <c r="S114" s="4"/>
@@ -17949,7 +17949,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId49"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId49"/>
   <headerFooter>
     <oddHeader>&amp;L資源タイプ語彙別表  &amp;P/&amp;N</oddHeader>
   </headerFooter>
@@ -22621,7 +22621,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId13"/>
   <headerFooter>
     <oddHeader>&amp;L語彙別表  &amp;P/&amp;N</oddHeader>
   </headerFooter>

</xml_diff>